<commit_message>
Added excel with results of test
</commit_message>
<xml_diff>
--- a/meetrapporten/working/Results.xlsx
+++ b/meetrapporten/working/Results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents-(D)\HBO-ICT\jaar2\Blok C\vision\HU-TI-1617C-Vision\meetrapporten\working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents-(D)\HBO-ICT\git\HBO-ICT\Jaar2\HU-TI-1617C-Vision\meetrapporten\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
   <si>
     <t>Single Color Channel</t>
   </si>
@@ -43,11 +43,20 @@
   <si>
     <t>Luminace</t>
   </si>
+  <si>
+    <t>Gemiddelden</t>
+  </si>
+  <si>
+    <t>Gemiddelde bij single color</t>
+  </si>
+  <si>
+    <t>Gemiddelde bij Luminace</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,8 +188,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -189,17 +199,15 @@
             <c:v>Female-1</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Blad1!$A$3:$A$52</c:f>
@@ -359,7 +367,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-583B-4CDD-9A7E-5FB36C34FB11}"/>
@@ -373,17 +380,15 @@
             <c:v>Child-1</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Blad1!$C$3:$C$52</c:f>
@@ -543,7 +548,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-583B-4CDD-9A7E-5FB36C34FB11}"/>
@@ -557,17 +561,15 @@
             <c:v>Male-2</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Blad1!$E$3:$E$52</c:f>
@@ -727,7 +729,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-583B-4CDD-9A7E-5FB36C34FB11}"/>
@@ -741,17 +742,15 @@
             <c:v>Male-3</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Blad1!$G$3:$G$52</c:f>
@@ -911,7 +910,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-583B-4CDD-9A7E-5FB36C34FB11}"/>
@@ -926,10 +924,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="1040157312"/>
         <c:axId val="1032217888"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="1040157312"/>
         <c:scaling>
@@ -3544,7 +3542,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3582,7 +3580,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3688,7 +3686,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3837,11 +3835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5190,7 +5188,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>354</v>
       </c>
@@ -5218,7 +5216,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>354</v>
       </c>
@@ -5246,7 +5244,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>374</v>
       </c>
@@ -5274,7 +5272,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>356</v>
       </c>
@@ -5302,18 +5300,151 @@
         <v>354</v>
       </c>
     </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P57" s="2"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f>SUM(A3:A52)/50</f>
+        <v>361.64</v>
+      </c>
+      <c r="C58">
+        <f>SUM(C3:C52)/50</f>
+        <v>353.16</v>
+      </c>
+      <c r="E58">
+        <f>SUM(E3:E52)/50</f>
+        <v>356.56</v>
+      </c>
+      <c r="G58">
+        <f>SUM(G3:G52)/50</f>
+        <v>363.86</v>
+      </c>
+      <c r="I58">
+        <f>SUM(I3:I52)/50</f>
+        <v>363.3</v>
+      </c>
+      <c r="K58">
+        <f>SUM(K3:K52)/50</f>
+        <v>358.6</v>
+      </c>
+      <c r="M58">
+        <f>SUM(M3:M52)/50</f>
+        <v>360.36</v>
+      </c>
+      <c r="O58">
+        <f>SUM(O3:O52)/50</f>
+        <v>366.62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f>SUM(A58,C58,E58,G58)/4</f>
+        <v>358.80499999999995</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I63">
+        <f>SUM(I58,K58,M58,O58)/4</f>
+        <v>362.22</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="23">
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:H56"/>
+    <mergeCell ref="I56:P56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="I1:P1"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:P2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
new push of results
</commit_message>
<xml_diff>
--- a/meetrapporten/working/Results.xlsx
+++ b/meetrapporten/working/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koend\Documents\GitHub\HU-TI-1617C-Vision\meetrapporten\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C493B5-0359-4F10-AA35-C55148F5A5C5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0D4021-90A9-4973-8D2A-AF30A0BD839A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17258" windowHeight="5663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>Single Color Channel</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Gemiddelde bij Standaard</t>
+  </si>
+  <si>
+    <t>blablabla</t>
   </si>
 </sst>
 </file>
@@ -3843,10 +3846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X63"/>
+  <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6104,29 +6107,13 @@
         <v>365.92500000000001</v>
       </c>
     </row>
+    <row r="71" spans="19:19" x14ac:dyDescent="0.45">
+      <c r="S71" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="Q62:S62"/>
-    <mergeCell ref="Q56:X56"/>
-    <mergeCell ref="Q57:R57"/>
-    <mergeCell ref="S57:T57"/>
-    <mergeCell ref="U57:V57"/>
-    <mergeCell ref="W57:X57"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q1:X1"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="I62:K62"/>
     <mergeCell ref="A55:B55"/>
@@ -6140,6 +6127,27 @@
     <mergeCell ref="K57:L57"/>
     <mergeCell ref="M57:N57"/>
     <mergeCell ref="O57:P57"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q1:X1"/>
+    <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="Q56:X56"/>
+    <mergeCell ref="Q57:R57"/>
+    <mergeCell ref="S57:T57"/>
+    <mergeCell ref="U57:V57"/>
+    <mergeCell ref="W57:X57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added final version of documents
</commit_message>
<xml_diff>
--- a/meetrapporten/working/Results.xlsx
+++ b/meetrapporten/working/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koend\Documents\GitHub\HU-TI-1617C-Vision\meetrapporten\working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents-(D)\HBO-ICT\git\HBO-ICT\Jaar2\HU-TI-1617C-Vision\meetrapporten\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCA9BCF-7680-4BD0-B1E4-8E7B714BA763}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743E4F55-B6A5-42CC-9A9C-3D7085080A29}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17258" windowHeight="5663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -96,8 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -106,7 +109,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -124,7 +127,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -994,7 +997,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1860,7 +1863,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2721,7 +2724,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3582,7 +3585,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3732,6 +3735,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Female-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Child-1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Male-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Male-3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>(Blad1!$A$58,Blad1!$C$58,Blad1!$E$58,Blad1!$G$58)</c:f>
@@ -3836,6 +3859,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Female-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Child-1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Male-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Male-3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>(Blad1!$I$58,Blad1!$K$58,Blad1!$M$58,Blad1!$O$58)</c:f>
@@ -3941,6 +3984,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Female-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Child-1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Male-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Male-3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>(Blad1!$Q$58,Blad1!$S$58,Blad1!$U$58,Blad1!$W$58)</c:f>
@@ -4060,6 +4123,32 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
                     <c:extLst>
@@ -4144,7 +4233,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4163,9 +4252,35 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Blad1!$E$58</c15:sqref>
@@ -4181,7 +4296,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-97B6-4EFB-97ED-4D48355D1944}"/>
                   </c:ext>
@@ -4247,7 +4362,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4266,9 +4381,35 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Blad1!$G$58</c15:sqref>
@@ -4284,7 +4425,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-97B6-4EFB-97ED-4D48355D1944}"/>
                   </c:ext>
@@ -4350,7 +4491,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4369,9 +4510,35 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Blad1!$K$58</c15:sqref>
@@ -4387,7 +4554,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-97B6-4EFB-97ED-4D48355D1944}"/>
                   </c:ext>
@@ -4454,7 +4621,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4473,9 +4640,35 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Blad1!$M$58</c15:sqref>
@@ -4491,7 +4684,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-97B6-4EFB-97ED-4D48355D1944}"/>
                   </c:ext>
@@ -4558,7 +4751,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4577,9 +4770,35 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Blad1!$O$58</c15:sqref>
@@ -4595,7 +4814,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-97B6-4EFB-97ED-4D48355D1944}"/>
                   </c:ext>
@@ -4662,7 +4881,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4681,9 +4900,35 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Blad1!$S$58</c15:sqref>
@@ -4699,7 +4944,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-97B6-4EFB-97ED-4D48355D1944}"/>
                   </c:ext>
@@ -4766,7 +5011,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4785,9 +5030,35 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Blad1!$U$58</c15:sqref>
@@ -4803,7 +5074,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-97B6-4EFB-97ED-4D48355D1944}"/>
                   </c:ext>
@@ -4870,7 +5141,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4889,9 +5160,35 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Blad1!$A$57,Blad1!$C$57,Blad1!$E$57,Blad1!$G$57)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>Female-1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Child-1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Male-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Male-3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Blad1!$W$58</c15:sqref>
@@ -4907,7 +5204,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-97B6-4EFB-97ED-4D48355D1944}"/>
                   </c:ext>
@@ -4922,12 +5219,45 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="537944040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -4940,7 +5270,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -4969,9 +5299,36 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="537942400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -8036,7 +8393,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9192,99 +9549,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J18" zoomScale="33" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="H69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2" t="s">
+      <c r="R2" s="3"/>
+      <c r="S2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
+      <c r="T2" s="3"/>
+      <c r="U2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2" t="s">
+      <c r="V2" s="3"/>
+      <c r="W2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="2"/>
+      <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>356</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="1">
         <v>350</v>
       </c>
@@ -9320,11 +9677,11 @@
         <v>431</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>357</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1">
         <v>361</v>
       </c>
@@ -9360,11 +9717,11 @@
         <v>376</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>370</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="1">
         <v>350</v>
       </c>
@@ -9400,11 +9757,11 @@
         <v>378</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>368</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1">
         <v>348</v>
       </c>
@@ -9440,11 +9797,11 @@
         <v>377</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>364</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1">
         <v>354</v>
       </c>
@@ -9480,11 +9837,11 @@
         <v>374</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>369</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="1">
         <v>348</v>
       </c>
@@ -9520,11 +9877,11 @@
         <v>382</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>373</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="1">
         <v>352</v>
       </c>
@@ -9560,11 +9917,11 @@
         <v>385</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>365</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1">
         <v>366</v>
       </c>
@@ -9600,11 +9957,11 @@
         <v>401</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>357</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="1">
         <v>352</v>
       </c>
@@ -9640,11 +9997,11 @@
         <v>381</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>363</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1">
         <v>349</v>
       </c>
@@ -9680,11 +10037,11 @@
         <v>377</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>361</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1">
         <v>352</v>
       </c>
@@ -9720,11 +10077,11 @@
         <v>378</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A14" s="1">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>358</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1">
         <v>350</v>
       </c>
@@ -9760,11 +10117,11 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>363</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1">
         <v>353</v>
       </c>
@@ -9800,11 +10157,11 @@
         <v>388</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A16" s="1">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>362</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1">
         <v>350</v>
       </c>
@@ -9840,11 +10197,11 @@
         <v>385</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A17" s="1">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
         <v>367</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="1">
         <v>361</v>
       </c>
@@ -9880,11 +10237,11 @@
         <v>375</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A18" s="1">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
         <v>358</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="1">
         <v>352</v>
       </c>
@@ -9920,11 +10277,11 @@
         <v>377</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A19" s="1">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>357</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1">
         <v>357</v>
       </c>
@@ -9960,11 +10317,11 @@
         <v>382</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A20" s="1">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>362</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="1">
         <v>361</v>
       </c>
@@ -10000,11 +10357,11 @@
         <v>379</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>357</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1">
         <v>352</v>
       </c>
@@ -10040,11 +10397,11 @@
         <v>390</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>358</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="1">
         <v>348</v>
       </c>
@@ -10080,11 +10437,11 @@
         <v>367</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>362</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="1">
         <v>353</v>
       </c>
@@ -10120,11 +10477,11 @@
         <v>373</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A24" s="1">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>357</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="1">
         <v>351</v>
       </c>
@@ -10160,11 +10517,11 @@
         <v>387</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A25" s="1">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>358</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="1">
         <v>353</v>
       </c>
@@ -10200,11 +10557,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A26" s="1">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
         <v>362</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="1">
         <v>353</v>
       </c>
@@ -10240,11 +10597,11 @@
         <v>359</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A27" s="1">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>357</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="1">
         <v>351</v>
       </c>
@@ -10280,11 +10637,11 @@
         <v>372</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>361</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="1">
         <v>350</v>
       </c>
@@ -10320,11 +10677,11 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A29" s="1">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>362</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="2"/>
       <c r="C29" s="1">
         <v>349</v>
       </c>
@@ -10360,11 +10717,11 @@
         <v>359</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A30" s="1">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>362</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="1">
         <v>344</v>
       </c>
@@ -10400,11 +10757,11 @@
         <v>359</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A31" s="1">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
         <v>356</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="1">
         <v>362</v>
       </c>
@@ -10440,11 +10797,11 @@
         <v>360</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A32" s="1">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>358</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="2"/>
       <c r="C32" s="1">
         <v>353</v>
       </c>
@@ -10480,11 +10837,11 @@
         <v>357</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A33" s="1">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>370</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="1">
         <v>353</v>
       </c>
@@ -10520,11 +10877,11 @@
         <v>354</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A34" s="1">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>364</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="1">
         <v>351</v>
       </c>
@@ -10560,11 +10917,11 @@
         <v>366</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A35" s="1">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
         <v>355</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="1">
         <v>350</v>
       </c>
@@ -10600,11 +10957,11 @@
         <v>356</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A36" s="1">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>358</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="1">
         <v>353</v>
       </c>
@@ -10640,11 +10997,11 @@
         <v>355</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A37" s="1">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>368</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="1">
         <v>352</v>
       </c>
@@ -10680,11 +11037,11 @@
         <v>359</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A38" s="1">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>394</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="1">
         <v>366</v>
       </c>
@@ -10720,11 +11077,11 @@
         <v>434</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>354</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="1">
         <v>363</v>
       </c>
@@ -10760,7 +11117,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>355</v>
       </c>
@@ -10800,7 +11157,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>362</v>
       </c>
@@ -10840,7 +11197,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>358</v>
       </c>
@@ -10880,7 +11237,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>365</v>
       </c>
@@ -10920,7 +11277,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>359</v>
       </c>
@@ -10960,7 +11317,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>355</v>
       </c>
@@ -11000,7 +11357,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>361</v>
       </c>
@@ -11040,7 +11397,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>366</v>
       </c>
@@ -11080,7 +11437,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>360</v>
       </c>
@@ -11120,7 +11477,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>354</v>
       </c>
@@ -11160,7 +11517,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>354</v>
       </c>
@@ -11200,7 +11557,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>374</v>
       </c>
@@ -11240,7 +11597,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>356</v>
       </c>
@@ -11280,95 +11637,95 @@
         <v>356</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="2"/>
+      <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2" t="s">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-      <c r="Q56" s="2" t="s">
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R56" s="2"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="2"/>
-      <c r="U56" s="2"/>
-      <c r="V56" s="2"/>
-      <c r="W56" s="2"/>
-      <c r="X56" s="2"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A57" s="2" t="s">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2" t="s">
+      <c r="D57" s="3"/>
+      <c r="E57" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2" t="s">
+      <c r="F57" s="3"/>
+      <c r="G57" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2" t="s">
+      <c r="H57" s="3"/>
+      <c r="I57" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2" t="s">
+      <c r="J57" s="3"/>
+      <c r="K57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2" t="s">
+      <c r="L57" s="3"/>
+      <c r="M57" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2" t="s">
+      <c r="N57" s="3"/>
+      <c r="O57" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2" t="s">
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R57" s="2"/>
-      <c r="S57" s="2" t="s">
+      <c r="R57" s="3"/>
+      <c r="S57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T57" s="2"/>
-      <c r="U57" s="2" t="s">
+      <c r="T57" s="3"/>
+      <c r="U57" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V57" s="2"/>
-      <c r="W57" s="2" t="s">
+      <c r="V57" s="3"/>
+      <c r="W57" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X57" s="2"/>
+      <c r="X57" s="3"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58">
         <f>SUM(A3:A52)/50</f>
         <v>361.64</v>
@@ -11418,30 +11775,30 @@
         <v>370.82</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A61" s="2" t="s">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62">
         <f>SUM(A58,C58,E58,G58)/4</f>
         <v>358.80499999999995</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="I62" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="Q62" s="2" t="s">
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="Q62" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R62" s="2"/>
-      <c r="S62" s="2"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="I63">
         <f>SUM(I58,K58,M58,O58)/4</f>
         <v>362.22</v>
@@ -11451,7 +11808,7 @@
         <v>365.92500000000001</v>
       </c>
     </row>
-    <row r="71" spans="19:19" x14ac:dyDescent="0.45">
+    <row r="71" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S71" t="s">
         <v>11</v>
       </c>

</xml_diff>